<commit_message>
update schedule, android first
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houser/Library/Mobile Documents/com~apple~CloudDocs/cos470/usm-cos470.github.io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houser/Google Drive/Courses/cos470/COS470 2022 Spring (Mobile)/usm-cos470.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AE617B-50AB-8F49-9249-573A6E7D96C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4DBB5D-9AA1-3F49-9C0D-B947BEDBE64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12700" yWindow="7080" windowWidth="24520" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12700" yWindow="4160" windowWidth="25360" windowHeight="22760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -136,19 +147,19 @@
     <t>[Fluid UI Wireframing](https://www.fluidui.com/editor/live/), [Planning Screens and their Relationships](https://developer.android.com/training/design-navigation/screen-planning.html)</t>
   </si>
   <si>
-    <t>[Project 2 - Android Due](/projects/project-2-android-tasklist)</t>
-  </si>
-  <si>
-    <t>[Project 1 - iOS Due](/projects/project-1-ios-tasklist)</t>
-  </si>
-  <si>
     <t>[Project 0 - GitHub Due](/projects/project-0-github)</t>
   </si>
   <si>
-    <t>[Project 3 - Hybrid Due](/projects/project-3-react-native-tasklist)</t>
-  </si>
-  <si>
     <t>[Project 4 - Your App Here](/projects/poject-4-student-choice)</t>
+  </si>
+  <si>
+    <t>[Project 2 - iOS Due](/projects/ios-tasklist)</t>
+  </si>
+  <si>
+    <t>[Project 1 - Android Due](/projects/android-tasklist)</t>
+  </si>
+  <si>
+    <t>[Project 3 - Hybrid Due](/projects/hybrid-tasklist)</t>
   </si>
 </sst>
 </file>
@@ -526,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,11 +579,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7">
         <f>DATE(2020,A2,B2)+TIME(5, 35,0)</f>
-        <v>43852.232638888891</v>
+        <v>43849.232638888891</v>
       </c>
       <c r="D2" s="8">
         <v>1</v>
@@ -584,136 +595,136 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" ref="C3:C18" si="0">DATE(2020,A3,B3)+TIME(5, 35,0)</f>
-        <v>43859.232638888891</v>
+        <v>43856.232638888891</v>
       </c>
       <c r="D3" s="8">
         <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="187" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7">
         <f t="shared" si="0"/>
-        <v>43866.232638888891</v>
+        <v>43863.232638888891</v>
       </c>
       <c r="D4" s="8">
         <v>3</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>2</v>
       </c>
       <c r="B5" s="6">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="0"/>
-        <v>43873.232638888891</v>
+        <v>43870.232638888891</v>
       </c>
       <c r="D5" s="8">
         <v>4</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="8" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>2</v>
       </c>
       <c r="B6" s="6">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7">
         <f t="shared" si="0"/>
-        <v>43880.232638888891</v>
+        <v>43877.232638888891</v>
       </c>
       <c r="D6" s="8">
         <v>5</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="187" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>2</v>
       </c>
       <c r="B7" s="6">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>43887.232638888891</v>
+        <v>43884.232638888891</v>
       </c>
       <c r="D7" s="8">
         <v>6</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>3</v>
       </c>
       <c r="B8" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="7">
         <f t="shared" si="0"/>
-        <v>43894.232638888891</v>
+        <v>43892.232638888891</v>
       </c>
       <c r="D8" s="8">
         <v>7</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -721,11 +732,11 @@
         <v>3</v>
       </c>
       <c r="B9" s="6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" si="0"/>
-        <v>43901.232638888891</v>
+        <v>43899.232638888891</v>
       </c>
       <c r="D9" s="8">
         <v>8</v>
@@ -737,7 +748,7 @@
         <v>31</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -745,11 +756,11 @@
         <v>3</v>
       </c>
       <c r="B10" s="6">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" si="0"/>
-        <v>43908.232638888891</v>
+        <v>43906.232638888891</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>34</v>
@@ -760,11 +771,11 @@
         <v>3</v>
       </c>
       <c r="B11" s="6">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>43915.232638888891</v>
+        <v>43913.232638888891</v>
       </c>
       <c r="D11" s="8">
         <v>9</v>
@@ -778,14 +789,14 @@
     </row>
     <row r="12" spans="1:7" s="8" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="6">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" si="0"/>
-        <v>43922.232638888891</v>
+        <v>43920.232638888891</v>
       </c>
       <c r="D12" s="8">
         <v>10</v>
@@ -802,11 +813,11 @@
         <v>4</v>
       </c>
       <c r="B13" s="6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="7">
         <f t="shared" si="0"/>
-        <v>43929.232638888891</v>
+        <v>43927.232638888891</v>
       </c>
       <c r="D13" s="8">
         <v>11</v>
@@ -823,11 +834,11 @@
         <v>4</v>
       </c>
       <c r="B14" s="6">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="7">
         <f t="shared" si="0"/>
-        <v>43936.232638888891</v>
+        <v>43934.232638888891</v>
       </c>
       <c r="D14" s="8">
         <v>12</v>
@@ -839,7 +850,7 @@
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -847,11 +858,11 @@
         <v>4</v>
       </c>
       <c r="B15" s="6">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>43943.232638888891</v>
+        <v>43941.232638888891</v>
       </c>
       <c r="D15" s="8">
         <v>13</v>
@@ -868,11 +879,11 @@
         <v>4</v>
       </c>
       <c r="B16" s="6">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>43950.232638888891</v>
+        <v>43948.232638888891</v>
       </c>
       <c r="D16" s="8">
         <v>14</v>
@@ -887,11 +898,11 @@
         <v>5</v>
       </c>
       <c r="B17" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C17" s="7">
         <f t="shared" si="0"/>
-        <v>43957.232638888891</v>
+        <v>43955.232638888891</v>
       </c>
       <c r="D17" s="8">
         <v>15</v>
@@ -906,11 +917,11 @@
         <v>5</v>
       </c>
       <c r="B18" s="6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="7">
         <f t="shared" si="0"/>
-        <v>43964.232638888891</v>
+        <v>43962.232638888891</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>7</v>
@@ -920,7 +931,7 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>